<commit_message>
verifying correlations and multicollinearity
</commit_message>
<xml_diff>
--- a/output/Correlation of all variables year 1.xlsx
+++ b/output/Correlation of all variables year 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Noa/Documents/Documents - MacBook Air/PhD/R:Stats:GIS/RStudio/R_Workspace/Pheromone_trap_code/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE2FE33-3B7B-A649-8F79-5C7104C30900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332CE525-B7AE-1544-933C-C00E48B86145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12760" yWindow="500" windowWidth="15960" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12760" yWindow="500" windowWidth="15960" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Correlation of all va" sheetId="1" r:id="rId1"/>
@@ -59,8 +59,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -256,37 +257,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1422,150 +1423,150 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="19.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="11" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="11">
         <v>-0.248529109435737</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="11">
         <v>1.17776525086051E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="12">
         <v>-0.31070174909299197</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="12">
         <v>1.4813645099397499E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="12">
         <v>-0.35477136653889002</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="12">
         <v>2.5358399630947799E-4</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="12">
         <v>-0.13474267790023001</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="12">
         <v>0.176942553348647</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="12">
         <v>0.90183033102529597</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="12">
         <v>3.1784266584167801E-38</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="12">
         <v>-0.14536510118168899</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="12">
         <v>0.14490200557757099</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="12">
         <v>9.9502037857151504E-3</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="12">
         <v>0.92093496792738205</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="12">
         <v>-0.48671844036303902</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="12">
         <v>2.1379971511608099E-7</v>
       </c>
     </row>

</xml_diff>